<commit_message>
"Updated with Notice Page Functionlaity "
</commit_message>
<xml_diff>
--- a/src/main/java/config/dataFile.xlsx
+++ b/src/main/java/config/dataFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aviraj/eclipse-workspace/DEMO_CRED/src/main/java/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aviraj/git/CredPortfolio1/src/main/java/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{F23DFF52-78CE-4948-9136-0B3C7EE570E5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{C7318A10-1EBB-1746-A2D9-7592C1D18C04}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="15800" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="500"/>
   </bookViews>
@@ -29,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Test_Loan_11</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TestCase</t>
   </si>
@@ -49,13 +46,13 @@
     <t>loan</t>
   </si>
   <si>
-    <t>TC002_CheckData</t>
-  </si>
-  <si>
     <t>minionadmin@yopmail.com</t>
   </si>
   <si>
     <t>Test@123</t>
+  </si>
+  <si>
+    <t>TC003_File_Upload</t>
   </si>
 </sst>
 </file>
@@ -469,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:HF3001"/>
+  <dimension ref="A1:HF3000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,36 +488,33 @@
   <sheetData>
     <row r="1" spans="1:213" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
+    </row>
+    <row ht="19" r="2" spans="1:213" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row ht="19" r="2" spans="1:213" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="N2" s="2"/>
       <c r="P2" s="6"/>
@@ -532,11 +526,16 @@
       <c r="CN2" s="1"/>
       <c r="CR2" s="1"/>
       <c r="DA2" s="1"/>
-      <c r="DD2" s="1"/>
       <c r="DH2" s="6"/>
       <c r="DM2" s="6"/>
       <c r="DR2" s="6"/>
       <c r="DW2" s="6"/>
+      <c r="EU2" s="2"/>
+      <c r="GI2" s="1"/>
+      <c r="GQ2" s="2"/>
+      <c r="GR2" s="1"/>
+      <c r="GV2" s="1"/>
+      <c r="HE2" s="1"/>
     </row>
     <row ht="19" r="3" spans="1:213" x14ac:dyDescent="0.2">
       <c r="D3" s="2"/>
@@ -554,12 +553,6 @@
       <c r="DM3" s="6"/>
       <c r="DR3" s="6"/>
       <c r="DW3" s="6"/>
-      <c r="EU3" s="2"/>
-      <c r="GI3" s="1"/>
-      <c r="GQ3" s="2"/>
-      <c r="GR3" s="1"/>
-      <c r="GV3" s="1"/>
-      <c r="HE3" s="1"/>
     </row>
     <row ht="19" r="4" spans="1:213" x14ac:dyDescent="0.2">
       <c r="D4" s="2"/>
@@ -595,22 +588,11 @@
       <c r="DR5" s="6"/>
       <c r="DW5" s="6"/>
     </row>
-    <row ht="19" r="6" spans="1:213" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:213" x14ac:dyDescent="0.2">
       <c r="D6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="5"/>
-      <c r="S6" s="1"/>
-      <c r="AQ6" s="2"/>
-      <c r="CE6" s="1"/>
-      <c r="CM6" s="2"/>
-      <c r="CN6" s="1"/>
+      <c r="Q6" s="4"/>
       <c r="CR6" s="1"/>
       <c r="DA6" s="1"/>
-      <c r="DH6" s="6"/>
-      <c r="DM6" s="6"/>
-      <c r="DR6" s="6"/>
-      <c r="DW6" s="6"/>
     </row>
     <row r="7" spans="1:213" x14ac:dyDescent="0.2">
       <c r="D7" s="2"/>
@@ -718,11 +700,9 @@
       <c r="D24" s="2"/>
       <c r="Q24" s="4"/>
       <c r="CR24" s="1"/>
-      <c r="DA24" s="1"/>
     </row>
     <row r="25" spans="4:105" x14ac:dyDescent="0.2">
       <c r="D25" s="2"/>
-      <c r="Q25" s="4"/>
       <c r="CR25" s="1"/>
     </row>
     <row r="26" spans="4:105" x14ac:dyDescent="0.2">
@@ -12625,16 +12605,11 @@
       <c r="D3000" s="2"/>
       <c r="CR3000" s="1"/>
     </row>
-    <row r="3001" spans="4:96" x14ac:dyDescent="0.2">
-      <c r="D3001" s="2"/>
-      <c r="CR3001" s="1"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2" xr:uid="{2F8C10B0-533F-6043-BB3A-250BF8EB61EA}"/>
-    <hyperlink r:id="rId2" ref="C2" xr:uid="{1EB4F2AB-F4FC-E744-A8AA-054AAAEEA1C2}"/>
-    <hyperlink display="https://dev.credgenics.com/app/customer-details?loan_id=Test_Loan_11&amp;company_id=ad8b5a88-637f-49a3-b8af-f341dd9db5fd&amp;trademark=Credgenics&amp;page=30" r:id="rId3" ref="E2" xr:uid="{A5DEBA95-230A-C744-A92E-E0223AE7C62E}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{ABBA1219-2BEA-7C4E-8F87-43CCB66E379B}"/>
+    <hyperlink r:id="rId2" ref="C2" xr:uid="{07597980-C175-8A4A-81CE-F8383B5EFD77}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>